<commit_message>
add DJI Air unit and RC Selector
</commit_message>
<xml_diff>
--- a/Pinmap.xlsx
+++ b/Pinmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyeonje\Desktop\Project\fc\STM32-FC-hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F7A57E-572C-4AFA-A907-1EC3E8F7CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FAEEEB-1609-4FAB-80B0-85D4696F74D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3855" windowWidth="29040" windowHeight="16440" xr2:uid="{0E7243C0-7080-495C-82E4-3D8F415C6423}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="666">
   <si>
     <t>PE2</t>
   </si>
@@ -1913,10 +1913,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PPM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TIM1_CH2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2181,6 +2177,30 @@
   </si>
   <si>
     <t>ADC123_IN11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPM_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_RED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_YELLO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_GREEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC_SEL0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC_SEL1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2691,9 +2711,9 @@
   </sheetPr>
   <dimension ref="A1:S169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2764,7 +2784,7 @@
     </row>
     <row r="2" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>575</v>
@@ -2807,7 +2827,7 @@
     </row>
     <row r="3" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>576</v>
@@ -2852,7 +2872,7 @@
     </row>
     <row r="4" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>577</v>
@@ -2895,7 +2915,7 @@
     </row>
     <row r="5" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>578</v>
@@ -2938,7 +2958,7 @@
     </row>
     <row r="6" spans="1:19" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>523</v>
@@ -2979,7 +2999,7 @@
     </row>
     <row r="7" spans="1:19" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>565</v>
@@ -3018,7 +3038,7 @@
     </row>
     <row r="8" spans="1:19" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>567</v>
@@ -3061,7 +3081,7 @@
     </row>
     <row r="9" spans="1:19" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>566</v>
@@ -3104,10 +3124,10 @@
     </row>
     <row r="10" spans="1:19" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>59</v>
@@ -3147,7 +3167,7 @@
     </row>
     <row r="11" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>569</v>
@@ -3186,7 +3206,7 @@
     </row>
     <row r="12" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>568</v>
@@ -3223,7 +3243,7 @@
     </row>
     <row r="13" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>571</v>
@@ -3262,7 +3282,7 @@
     </row>
     <row r="14" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>572</v>
@@ -3712,10 +3732,10 @@
     </row>
     <row r="26" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>141</v>
@@ -3757,10 +3777,10 @@
     </row>
     <row r="27" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>148</v>
@@ -3802,7 +3822,7 @@
     </row>
     <row r="28" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>589</v>
@@ -3845,7 +3865,7 @@
     </row>
     <row r="29" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>590</v>
@@ -3972,10 +3992,10 @@
     </row>
     <row r="32" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>176</v>
@@ -4050,10 +4070,10 @@
     </row>
     <row r="34" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>186</v>
@@ -4087,10 +4107,10 @@
     </row>
     <row r="35" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>188</v>
@@ -4124,10 +4144,10 @@
     </row>
     <row r="36" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>193</v>
@@ -4161,10 +4181,10 @@
     </row>
     <row r="37" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>657</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>658</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>197</v>
@@ -4320,7 +4340,7 @@
     </row>
     <row r="42" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>223</v>
@@ -4363,7 +4383,7 @@
     </row>
     <row r="43" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>231</v>
@@ -4410,7 +4430,7 @@
     </row>
     <row r="44" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>235</v>
@@ -4453,7 +4473,7 @@
     </row>
     <row r="45" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>240</v>
@@ -4494,7 +4514,7 @@
     </row>
     <row r="46" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>244</v>
@@ -4535,7 +4555,7 @@
     </row>
     <row r="47" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="11" t="s">
@@ -4587,7 +4607,7 @@
     </row>
     <row r="49" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="2" t="s">
@@ -4680,13 +4700,13 @@
     </row>
     <row r="52" spans="1:19" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>255</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>253</v>
@@ -5082,7 +5102,7 @@
     </row>
     <row r="64" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>305</v>
@@ -5117,7 +5137,7 @@
     </row>
     <row r="65" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>308</v>
@@ -5152,7 +5172,7 @@
     </row>
     <row r="66" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>296</v>
@@ -5193,7 +5213,7 @@
     </row>
     <row r="67" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>300</v>
@@ -5230,7 +5250,7 @@
     </row>
     <row r="68" spans="1:19" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>303</v>
@@ -5271,10 +5291,10 @@
     </row>
     <row r="69" spans="1:19" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>1</v>
@@ -5306,7 +5326,7 @@
     </row>
     <row r="70" spans="1:19" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>310</v>
@@ -5347,7 +5367,7 @@
     </row>
     <row r="71" spans="1:19" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>315</v>
@@ -5390,7 +5410,7 @@
     </row>
     <row r="72" spans="1:19" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>321</v>
@@ -5437,7 +5457,7 @@
     </row>
     <row r="73" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>326</v>
@@ -5474,7 +5494,7 @@
     </row>
     <row r="74" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>330</v>
@@ -5511,7 +5531,7 @@
     </row>
     <row r="75" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>334</v>
@@ -5548,7 +5568,7 @@
     </row>
     <row r="76" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>338</v>
@@ -5585,10 +5605,10 @@
     </row>
     <row r="77" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>593</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>594</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>341</v>
@@ -5928,7 +5948,7 @@
     </row>
     <row r="88" spans="1:19" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>369</v>
@@ -5967,7 +5987,7 @@
     </row>
     <row r="89" spans="1:19" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B89" s="14" t="s">
         <v>371</v>
@@ -6006,7 +6026,7 @@
     </row>
     <row r="90" spans="1:19" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B90" s="14" t="s">
         <v>373</v>
@@ -6043,7 +6063,7 @@
     </row>
     <row r="91" spans="1:19" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B91" s="14" t="s">
         <v>376</v>
@@ -6892,7 +6912,7 @@
     </row>
     <row r="118" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>155</v>
@@ -6925,7 +6945,7 @@
     </row>
     <row r="119" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>161</v>
@@ -6997,7 +7017,7 @@
     </row>
     <row r="121" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>55</v>
@@ -7036,7 +7056,7 @@
     </row>
     <row r="122" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>228</v>
@@ -7143,10 +7163,10 @@
     </row>
     <row r="125" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>445</v>
@@ -7182,7 +7202,7 @@
     </row>
     <row r="126" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>286</v>
@@ -7322,7 +7342,7 @@
     </row>
     <row r="130" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="2" t="s">
@@ -7394,7 +7414,7 @@
     </row>
     <row r="132" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="2" t="s">
@@ -7499,7 +7519,7 @@
     </row>
     <row r="135" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="2" t="s">
@@ -7536,7 +7556,7 @@
     </row>
     <row r="136" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="2" t="s">
@@ -7831,7 +7851,9 @@
       </c>
     </row>
     <row r="146" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="3"/>
+      <c r="A146" s="3" t="s">
+        <v>661</v>
+      </c>
       <c r="B146" s="3"/>
       <c r="C146" s="2" t="s">
         <v>482</v>
@@ -7858,7 +7880,9 @@
       </c>
     </row>
     <row r="147" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="3"/>
+      <c r="A147" s="3" t="s">
+        <v>662</v>
+      </c>
       <c r="B147" s="3"/>
       <c r="C147" s="2" t="s">
         <v>483</v>
@@ -7885,7 +7909,9 @@
       </c>
     </row>
     <row r="148" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="3"/>
+      <c r="A148" s="3" t="s">
+        <v>663</v>
+      </c>
       <c r="B148" s="3"/>
       <c r="C148" s="2" t="s">
         <v>484</v>
@@ -7912,7 +7938,9 @@
       </c>
     </row>
     <row r="149" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="3"/>
+      <c r="A149" s="3" t="s">
+        <v>664</v>
+      </c>
       <c r="B149" s="3"/>
       <c r="C149" s="2" t="s">
         <v>485</v>
@@ -7939,7 +7967,9 @@
       </c>
     </row>
     <row r="150" spans="1:19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="3"/>
+      <c r="A150" s="3" t="s">
+        <v>665</v>
+      </c>
       <c r="B150" s="3"/>
       <c r="C150" s="2" t="s">
         <v>486</v>

</xml_diff>